<commit_message>
panel data still fail
</commit_message>
<xml_diff>
--- a/additionalCityData.xlsx
+++ b/additionalCityData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\whistlaker\Documents\econometricIntro\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD80E32E-5A73-4C36-93B6-3CD917EC22E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4E6A1B-E660-4F36-A73D-8A653597E92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="34">
   <si>
     <t>就業者從業身分結構-受僱者(％)</t>
   </si>
@@ -129,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="#,##0_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -213,19 +213,19 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AV1" sqref="AV1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AO36" sqref="AO36:BI40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
@@ -3090,448 +3090,72 @@
     </row>
     <row r="26" spans="1:58" ht="16.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="27" spans="1:58" ht="16.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="1:58" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="K28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" t="s">
-        <v>12</v>
-      </c>
-      <c r="N28" t="s">
-        <v>13</v>
-      </c>
-      <c r="O28" t="s">
-        <v>14</v>
-      </c>
-      <c r="P28" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>16</v>
-      </c>
-      <c r="R28" t="s">
-        <v>17</v>
-      </c>
-      <c r="S28" t="s">
-        <v>18</v>
-      </c>
-      <c r="T28" t="s">
-        <v>19</v>
-      </c>
-      <c r="U28" t="s">
-        <v>20</v>
-      </c>
-      <c r="V28" t="s">
-        <v>21</v>
-      </c>
-      <c r="W28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X28" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.45">
-      <c r="J29">
-        <v>107</v>
-      </c>
-      <c r="K29">
-        <v>95.8</v>
-      </c>
-      <c r="L29">
-        <v>91.27</v>
-      </c>
-      <c r="M29">
-        <v>98.86</v>
-      </c>
-      <c r="N29">
-        <v>96.93</v>
-      </c>
-      <c r="O29">
-        <v>99.59</v>
-      </c>
-      <c r="P29">
-        <v>97.89</v>
-      </c>
-      <c r="Q29">
-        <v>102.15</v>
-      </c>
-      <c r="R29">
-        <v>104.31</v>
-      </c>
-      <c r="S29">
-        <v>106.58</v>
-      </c>
-      <c r="T29">
-        <v>103.75</v>
-      </c>
-      <c r="U29">
-        <v>104.98</v>
-      </c>
-      <c r="V29">
-        <v>107.61</v>
-      </c>
-      <c r="W29">
-        <v>108.14</v>
-      </c>
-      <c r="X29">
-        <v>104.37</v>
-      </c>
-      <c r="Y29">
-        <v>106.38</v>
-      </c>
-      <c r="Z29">
-        <v>102.81</v>
-      </c>
-      <c r="AA29">
-        <v>106.27</v>
-      </c>
-      <c r="AB29">
-        <v>99.89</v>
-      </c>
-      <c r="AC29">
-        <v>97.37</v>
-      </c>
-      <c r="AD29">
-        <v>94.36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.45">
-      <c r="J30">
-        <v>108</v>
-      </c>
-      <c r="K30">
-        <v>95.55</v>
-      </c>
-      <c r="L30">
-        <v>90.98</v>
-      </c>
-      <c r="M30">
-        <v>98.52</v>
-      </c>
-      <c r="N30">
-        <v>96.72</v>
-      </c>
-      <c r="O30">
-        <v>99.34</v>
-      </c>
-      <c r="P30">
-        <v>97.61</v>
-      </c>
-      <c r="Q30">
-        <v>101.9</v>
-      </c>
-      <c r="R30">
-        <v>104.25</v>
-      </c>
-      <c r="S30">
-        <v>106.48</v>
-      </c>
-      <c r="T30">
-        <v>103.53</v>
-      </c>
-      <c r="U30">
-        <v>104.68</v>
-      </c>
-      <c r="V30">
-        <v>107.41</v>
-      </c>
-      <c r="W30">
-        <v>108.01</v>
-      </c>
-      <c r="X30">
-        <v>104.1</v>
-      </c>
-      <c r="Y30">
-        <v>106.04</v>
-      </c>
-      <c r="Z30">
-        <v>102.42</v>
-      </c>
-      <c r="AA30">
-        <v>106.6</v>
-      </c>
-      <c r="AB30">
-        <v>99.67</v>
-      </c>
-      <c r="AC30">
-        <v>97.24</v>
-      </c>
-      <c r="AD30">
-        <v>94.12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.45">
-      <c r="J31">
-        <v>109</v>
-      </c>
-      <c r="K31">
-        <v>95.43</v>
-      </c>
-      <c r="L31">
-        <v>90.82</v>
-      </c>
-      <c r="M31">
-        <v>98.23</v>
-      </c>
-      <c r="N31">
-        <v>96.52</v>
-      </c>
-      <c r="O31">
-        <v>99.24</v>
-      </c>
-      <c r="P31">
-        <v>97.33</v>
-      </c>
-      <c r="Q31">
-        <v>101.58</v>
-      </c>
-      <c r="R31">
-        <v>104.29</v>
-      </c>
-      <c r="S31">
-        <v>106.35</v>
-      </c>
-      <c r="T31">
-        <v>103.37</v>
-      </c>
-      <c r="U31">
-        <v>104.51</v>
-      </c>
-      <c r="V31">
-        <v>107.16</v>
-      </c>
-      <c r="W31">
-        <v>107.82</v>
-      </c>
-      <c r="X31">
-        <v>103.85</v>
-      </c>
-      <c r="Y31">
-        <v>105.7</v>
-      </c>
-      <c r="Z31">
-        <v>102.3</v>
-      </c>
-      <c r="AA31">
-        <v>105.99</v>
-      </c>
-      <c r="AB31">
-        <v>99.47</v>
-      </c>
-      <c r="AC31">
-        <v>97.39</v>
-      </c>
-      <c r="AD31">
-        <v>93.69</v>
-      </c>
-    </row>
+    <row r="28" spans="1:58" ht="16.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="37" spans="41:60" x14ac:dyDescent="0.45">
-      <c r="AO37" s="3">
-        <v>22419</v>
-      </c>
-      <c r="AP37" s="3">
-        <v>28550</v>
-      </c>
-      <c r="AQ37" s="3">
-        <v>23049</v>
-      </c>
-      <c r="AR37" s="3">
-        <v>23267</v>
-      </c>
-      <c r="AS37" s="3">
-        <v>19536</v>
-      </c>
-      <c r="AT37" s="3">
-        <v>21674</v>
-      </c>
-      <c r="AU37" s="3">
-        <v>21174</v>
-      </c>
-      <c r="AV37" s="3">
-        <v>24784</v>
-      </c>
-      <c r="AW37" s="3">
-        <v>17965</v>
-      </c>
-      <c r="AX37" s="3">
-        <v>15929</v>
-      </c>
-      <c r="AY37" s="3">
-        <v>16637</v>
-      </c>
-      <c r="AZ37" s="3">
-        <v>17449</v>
-      </c>
-      <c r="BA37" s="3">
-        <v>18272</v>
-      </c>
-      <c r="BB37" s="3">
-        <v>18952</v>
-      </c>
-      <c r="BC37" s="3">
-        <v>17810</v>
-      </c>
-      <c r="BD37" s="3">
-        <v>19507</v>
-      </c>
-      <c r="BE37" s="3">
-        <v>17411</v>
-      </c>
-      <c r="BF37" s="3">
-        <v>21801</v>
-      </c>
-      <c r="BG37" s="3">
-        <v>26925</v>
-      </c>
-      <c r="BH37" s="7">
-        <v>20861</v>
-      </c>
+      <c r="AO37" s="3"/>
+      <c r="AP37" s="3"/>
+      <c r="AQ37" s="3"/>
+      <c r="AR37" s="3"/>
+      <c r="AS37" s="3"/>
+      <c r="AT37" s="3"/>
+      <c r="AU37" s="3"/>
+      <c r="AV37" s="3"/>
+      <c r="AW37" s="3"/>
+      <c r="AX37" s="3"/>
+      <c r="AY37" s="3"/>
+      <c r="AZ37" s="3"/>
+      <c r="BA37" s="3"/>
+      <c r="BB37" s="3"/>
+      <c r="BC37" s="3"/>
+      <c r="BD37" s="3"/>
+      <c r="BE37" s="3"/>
+      <c r="BF37" s="3"/>
+      <c r="BG37" s="3"/>
+      <c r="BH37" s="7"/>
     </row>
     <row r="38" spans="41:60" x14ac:dyDescent="0.45">
-      <c r="AO38" s="3">
-        <v>22755</v>
-      </c>
-      <c r="AP38" s="3">
-        <v>30981</v>
-      </c>
-      <c r="AQ38" s="3">
-        <v>22147</v>
-      </c>
-      <c r="AR38" s="3">
-        <v>24281</v>
-      </c>
-      <c r="AS38" s="3">
-        <v>20114</v>
-      </c>
-      <c r="AT38" s="3">
-        <v>22942</v>
-      </c>
-      <c r="AU38" s="3">
-        <v>21707</v>
-      </c>
-      <c r="AV38" s="3">
-        <v>24391</v>
-      </c>
-      <c r="AW38" s="3">
-        <v>18057</v>
-      </c>
-      <c r="AX38" s="3">
-        <v>17342</v>
-      </c>
-      <c r="AY38" s="3">
-        <v>17184</v>
-      </c>
-      <c r="AZ38" s="3">
-        <v>18114</v>
-      </c>
-      <c r="BA38" s="3">
-        <v>18046</v>
-      </c>
-      <c r="BB38" s="3">
-        <v>18372</v>
-      </c>
-      <c r="BC38" s="3">
-        <v>17457</v>
-      </c>
-      <c r="BD38" s="3">
-        <v>20041</v>
-      </c>
-      <c r="BE38" s="3">
-        <v>18883</v>
-      </c>
-      <c r="BF38" s="3">
-        <v>22324</v>
-      </c>
-      <c r="BG38" s="3">
-        <v>26703</v>
-      </c>
-      <c r="BH38" s="7">
-        <v>21417</v>
-      </c>
+      <c r="AO38" s="3"/>
+      <c r="AP38" s="3"/>
+      <c r="AQ38" s="3"/>
+      <c r="AR38" s="3"/>
+      <c r="AS38" s="3"/>
+      <c r="AT38" s="3"/>
+      <c r="AU38" s="3"/>
+      <c r="AV38" s="3"/>
+      <c r="AW38" s="3"/>
+      <c r="AX38" s="3"/>
+      <c r="AY38" s="3"/>
+      <c r="AZ38" s="3"/>
+      <c r="BA38" s="3"/>
+      <c r="BB38" s="3"/>
+      <c r="BC38" s="3"/>
+      <c r="BD38" s="3"/>
+      <c r="BE38" s="3"/>
+      <c r="BF38" s="3"/>
+      <c r="BG38" s="3"/>
+      <c r="BH38" s="7"/>
     </row>
     <row r="39" spans="41:60" x14ac:dyDescent="0.45">
-      <c r="AO39" s="3">
-        <v>23061</v>
-      </c>
-      <c r="AP39" s="3">
-        <v>30713</v>
-      </c>
-      <c r="AQ39" s="3">
-        <v>22537</v>
-      </c>
-      <c r="AR39" s="3">
-        <v>24187</v>
-      </c>
-      <c r="AS39" s="3">
-        <v>21019</v>
-      </c>
-      <c r="AT39" s="3">
-        <v>23159</v>
-      </c>
-      <c r="AU39" s="3">
-        <v>21383</v>
-      </c>
-      <c r="AV39" s="3">
-        <v>26661</v>
-      </c>
-      <c r="AW39" s="3">
-        <v>18739</v>
-      </c>
-      <c r="AX39" s="3">
-        <v>17794</v>
-      </c>
-      <c r="AY39" s="3">
-        <v>18874</v>
-      </c>
-      <c r="AZ39" s="3">
-        <v>18270</v>
-      </c>
-      <c r="BA39" s="3">
-        <v>19531</v>
-      </c>
-      <c r="BB39" s="3">
-        <v>19964</v>
-      </c>
-      <c r="BC39" s="3">
-        <v>18825</v>
-      </c>
-      <c r="BD39" s="3">
-        <v>19300</v>
-      </c>
-      <c r="BE39" s="3">
-        <v>19740</v>
-      </c>
-      <c r="BF39" s="3">
-        <v>22628</v>
-      </c>
-      <c r="BG39" s="3">
-        <v>26455</v>
-      </c>
-      <c r="BH39" s="7">
-        <v>21656</v>
-      </c>
+      <c r="AO39" s="3"/>
+      <c r="AP39" s="3"/>
+      <c r="AQ39" s="3"/>
+      <c r="AR39" s="3"/>
+      <c r="AS39" s="3"/>
+      <c r="AT39" s="3"/>
+      <c r="AU39" s="3"/>
+      <c r="AV39" s="3"/>
+      <c r="AW39" s="3"/>
+      <c r="AX39" s="3"/>
+      <c r="AY39" s="3"/>
+      <c r="AZ39" s="3"/>
+      <c r="BA39" s="3"/>
+      <c r="BB39" s="3"/>
+      <c r="BC39" s="3"/>
+      <c r="BD39" s="3"/>
+      <c r="BE39" s="3"/>
+      <c r="BF39" s="3"/>
+      <c r="BG39" s="3"/>
+      <c r="BH39" s="7"/>
     </row>
     <row r="75" spans="39:58" x14ac:dyDescent="0.45">
       <c r="AM75" s="3">

</xml_diff>